<commit_message>
refactor [FakturaController, twig templates] faktura strana razdvojena na stranu za prikaz i stranu za unos
</commit_message>
<xml_diff>
--- a/public/br1Faktura.xlsx
+++ b/public/br1Faktura.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Faktura</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Organizacija</t>
   </si>
   <si>
-    <t>Organizacija 3</t>
+    <t>Organizacija 1</t>
   </si>
   <si>
     <t>Stavke</t>
@@ -56,19 +56,22 @@
     <t>Iznos</t>
   </si>
   <si>
-    <t>Drvo</t>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Pesak</t>
   </si>
   <si>
     <t>m3</t>
   </si>
   <si>
-    <t>Pesak</t>
-  </si>
-  <si>
-    <t>Silikon</t>
-  </si>
-  <si>
-    <t>l</t>
+    <t>Stiropor</t>
+  </si>
+  <si>
+    <t>m2</t>
   </si>
   <si>
     <t>Ukupan iznos</t>
@@ -471,16 +474,16 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7">
-        <v>6.0</v>
+        <v>30.0</v>
       </c>
       <c r="E7">
-        <v>6.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -488,41 +491,41 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>15.2</v>
       </c>
       <c r="E8">
-        <v>60.8</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>2.0</v>
+        <v>20.1</v>
       </c>
       <c r="E9">
-        <v>12.0</v>
+        <v>20.1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="D10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>78.8</v>
+        <v>215.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>